<commit_message>
script for extraction conversion scores, saved in csv file
</commit_message>
<xml_diff>
--- a/manuscript/Table 1.xlsx
+++ b/manuscript/Table 1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\pathologie\PRL\Groep-Brosens\2. Anna Vera\2. ACN-SPN-NET\Pancreas-ID\manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{4C883341-86EB-432E-B207-EA60E2600F43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491487A8-FDE2-493B-87EC-5A7AC7540304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t xml:space="preserve">Dataset </t>
   </si>
@@ -105,9 +105,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Pancreatic Neuroendocrine Neoplasms</t>
-  </si>
-  <si>
     <t>GSE117852</t>
   </si>
   <si>
@@ -132,19 +129,16 @@
     <t>E-MTAB-7924</t>
   </si>
   <si>
-    <t>PanNETs</t>
-  </si>
-  <si>
-    <t>PanNECs</t>
-  </si>
-  <si>
     <t>JGAS000359</t>
+  </si>
+  <si>
+    <t>Pancreatic Neuroendocrine Carcinoma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -522,11 +516,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,12 +535,12 @@
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
@@ -555,7 +549,7 @@
       <c r="G3"/>
       <c r="H3"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -569,16 +563,16 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -601,7 +595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>25</v>
       </c>
@@ -621,12 +615,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>17</v>
@@ -635,21 +629,21 @@
         <v>20</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>17</v>
@@ -667,9 +661,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>17</v>
@@ -687,7 +681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
@@ -710,7 +704,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -724,16 +718,16 @@
         <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
         <v>22</v>
@@ -754,7 +748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="4" t="s">
         <v>22</v>
@@ -775,7 +769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -795,40 +789,46 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
       <c r="H15" s="5">
-        <v>43</v>
-      </c>
-      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
       <c r="H16" s="5">
-        <v>15</v>
-      </c>
-      <c r="I16" t="s">
-        <v>36</v>
-      </c>
-      <c r="J16">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjusted annotation file, minor changes to model training, and added some plots to FIGURE2
</commit_message>
<xml_diff>
--- a/manuscript/Table 1.xlsx
+++ b/manuscript/Table 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\pathologie\PRL\Groep-Brosens\2. Anna Vera\2. ACN-SPN-NET\Pancreas-ID\manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491487A8-FDE2-493B-87EC-5A7AC7540304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CE87AB-32DA-45B3-A493-9CBDE596D6A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t xml:space="preserve">Dataset </t>
   </si>
@@ -133,13 +133,16 @@
   </si>
   <si>
     <t>Pancreatic Neuroendocrine Carcinoma</t>
+  </si>
+  <si>
+    <t>EGAD00010001298</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +161,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -203,6 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -520,7 +531,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,12 +715,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>22</v>
+      <c r="C11" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>17</v>

</xml_diff>